<commit_message>
tracking table and exmple with friend
</commit_message>
<xml_diff>
--- a/tracking/Tracking.xlsx
+++ b/tracking/Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\myproject\BusAnalizer\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D49144A-5147-474D-AD33-8D6264EA2E8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11455813-0199-4789-8D9B-A21058CA9457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="420" windowWidth="27000" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="435" windowWidth="27000" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>13.05</t>
   </si>
@@ -54,9 +54,6 @@
     <t>cubeIDE instalat</t>
   </si>
   <si>
-    <t>ToDo</t>
-  </si>
-  <si>
     <t>-friend,functii lamda, clase statice</t>
   </si>
   <si>
@@ -76,6 +73,31 @@
   </si>
   <si>
     <t>-explicatii despre registri GPIO</t>
+  </si>
+  <si>
+    <t>27.05</t>
+  </si>
+  <si>
+    <t>ToDo BoTi</t>
+  </si>
+  <si>
+    <t>ToDo Team</t>
+  </si>
+  <si>
+    <t>clasa GPIO</t>
+  </si>
+  <si>
+    <t>start class GPIO, functia de initializare</t>
+  </si>
+  <si>
+    <t>clasa GPIO start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-rewrite GPIO driver in C++
+</t>
+  </si>
+  <si>
+    <t>-exemplu clasa friend</t>
   </si>
 </sst>
 </file>
@@ -91,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +132,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -143,11 +171,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -162,12 +203,26 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -445,7 +500,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,10 +509,11 @@
     <col min="3" max="4" width="41" customWidth="1"/>
     <col min="5" max="5" width="46.85546875" customWidth="1"/>
     <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
+      <c r="A1" s="7"/>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -471,10 +527,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -491,48 +550,62 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -592,7 +665,6 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>

</xml_diff>

<commit_message>
meeting minutes for weekly
</commit_message>
<xml_diff>
--- a/tracking/Tracking.xlsx
+++ b/tracking/Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\myproject\BusAnalizer\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11455813-0199-4789-8D9B-A21058CA9457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF0B152-39CF-437D-8CAF-4D8ED73DF368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="435" windowWidth="27000" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>13.05</t>
   </si>
@@ -54,9 +54,6 @@
     <t>cubeIDE instalat</t>
   </si>
   <si>
-    <t>-friend,functii lamda, clase statice</t>
-  </si>
-  <si>
     <t>20.05</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
   </si>
   <si>
     <t>clona proiect, clasa gpio inceputa</t>
-  </si>
-  <si>
-    <t>-explicatii despre registri GPIO</t>
   </si>
   <si>
     <t>27.05</t>
@@ -98,6 +92,28 @@
   </si>
   <si>
     <t>-exemplu clasa friend</t>
+  </si>
+  <si>
+    <t>04.06</t>
+  </si>
+  <si>
+    <t>exemplu friend, branch proiect, video</t>
+  </si>
+  <si>
+    <t>clasa GPIO, exemplu friend</t>
+  </si>
+  <si>
+    <t>branch, scheletul clasei, instantiere</t>
+  </si>
+  <si>
+    <t>-functii lamda, clase statice</t>
+  </si>
+  <si>
+    <t>Andrei: CAN
+Gabriel: USB
+Ana: Timer
+Alina:RTC
+GPIO pe branch</t>
   </si>
 </sst>
 </file>
@@ -500,7 +516,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,10 +543,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -550,68 +566,76 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>

</xml_diff>